<commit_message>
build files of the 20170413 zip
</commit_message>
<xml_diff>
--- a/publication/part1000/CR_210_1/Bugzilla_list.xlsx
+++ b/publication/part1000/CR_210_1/Bugzilla_list.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
+    <workbookView xWindow="4680" yWindow="-19160" windowWidth="24880" windowHeight="15280"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="369">
   <si>
     <t>d</t>
   </si>
@@ -1137,6 +1137,12 @@
   </si>
   <si>
     <t>Column3</t>
+  </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>added in April 2017 in 210_1</t>
   </si>
 </sst>
 </file>
@@ -1595,8 +1601,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:M149" totalsRowShown="0" headerRowDxfId="19">
-  <autoFilter ref="A1:M149">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:M150" totalsRowShown="0" headerRowDxfId="19">
+  <autoFilter ref="A1:M150">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -1926,21 +1932,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M149"/>
+  <dimension ref="A1:M150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L55" sqref="L55"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G152" sqref="G152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="4" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="17.5" style="4" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" style="19" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" style="19" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" style="7" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" style="19" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" style="19" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" style="7" customWidth="1"/>
     <col min="7" max="7" width="35.1640625" style="19" customWidth="1"/>
     <col min="8" max="8" width="5.6640625" style="4" customWidth="1"/>
     <col min="9" max="9" width="35.1640625" style="19" customWidth="1"/>
@@ -2962,7 +2968,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
         <v>3</v>
       </c>
@@ -3211,7 +3217,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="55" spans="1:12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>3</v>
       </c>
@@ -3333,7 +3339,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="60" spans="1:12" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>3</v>
       </c>
@@ -3671,7 +3677,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="128" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" ht="64" x14ac:dyDescent="0.2">
       <c r="A74" s="5">
         <v>3</v>
       </c>
@@ -3796,7 +3802,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="79" spans="1:12" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>3</v>
       </c>
@@ -4346,7 +4352,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="102" spans="1:13" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>3</v>
       </c>
@@ -4918,7 +4924,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="126" spans="1:12" ht="112" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A126" s="5">
         <v>3</v>
       </c>
@@ -5483,6 +5489,29 @@
         <v>282</v>
       </c>
       <c r="M149" s="12"/>
+    </row>
+    <row r="150" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A150" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="B150" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="C150" s="8"/>
+      <c r="D150" s="8"/>
+      <c r="E150" s="9"/>
+      <c r="F150" s="10"/>
+      <c r="G150" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="H150" s="9"/>
+      <c r="I150" s="9"/>
+      <c r="J150" s="9"/>
+      <c r="K150" s="11">
+        <v>5430</v>
+      </c>
+      <c r="L150" s="12"/>
+      <c r="M150" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>